<commit_message>
Updated exported files from PLIT_relcov_extraction
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/PLITs/plits_length_df.xlsx
+++ b/Multi-taxa_data/PLITs/plits_length_df.xlsx
@@ -504,19 +504,19 @@
         <v>2476</v>
       </c>
       <c r="C6">
-        <v>2649</v>
+        <v>2598</v>
       </c>
       <c r="D6">
-        <v>2722</v>
+        <v>2621</v>
       </c>
       <c r="E6">
-        <v>2554</v>
+        <v>2650</v>
       </c>
       <c r="F6">
-        <v>2685</v>
+        <v>2650</v>
       </c>
       <c r="G6">
-        <v>2720</v>
+        <v>2698</v>
       </c>
     </row>
     <row r="7">

</xml_diff>